<commit_message>
add ordinal encoder, fixed missing value cleaning
</commit_message>
<xml_diff>
--- a/Huimin/Variable_Analysis.xlsx
+++ b/Huimin/Variable_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop2\Documents\Bootcamp\Kaggle-House-Prices\Huimin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB8DAC1-339D-468F-AA21-DFFD42E51093}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084F8DD2-798E-480B-9CA4-71F2D91B3C46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="1470" windowWidth="17910" windowHeight="11385" xr2:uid="{62575EAA-3102-4243-B684-290054381A1F}"/>
   </bookViews>
@@ -833,7 +833,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>